<commit_message>
DATA: data for 2nd revision
</commit_message>
<xml_diff>
--- a/data/basisSetSizes.xlsx
+++ b/data/basisSetSizes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morgunov/vv/cebe_prediction/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morgunov/vv/cebe_prediction/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63B6D92-DEA1-2D4B-AD90-47BBCE585C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5AB5EE-4200-1540-8979-470B9946B46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="73">
   <si>
     <t>H</t>
   </si>
@@ -246,6 +246,12 @@
   </si>
   <si>
     <t># Func</t>
+  </si>
+  <si>
+    <t>Num. Functions</t>
+  </si>
+  <si>
+    <t>Contraction</t>
   </si>
 </sst>
 </file>
@@ -282,7 +288,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -305,24 +311,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -663,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:V23"/>
+  <dimension ref="B3:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3:X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -680,17 +676,18 @@
     <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.6640625" customWidth="1"/>
     <col min="20" max="20" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="C3" s="6" t="s">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="6"/>
       <c r="I3" s="2" t="s">
         <v>2</v>
       </c>
@@ -715,19 +712,27 @@
       <c r="Q3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="R3" s="4"/>
+      <c r="R3" s="3"/>
       <c r="S3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="V3" s="3"/>
-    </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -769,7 +774,7 @@
       <c r="Q4" s="1">
         <v>14</v>
       </c>
-      <c r="R4" s="5"/>
+      <c r="R4" s="4"/>
       <c r="S4" s="1" t="s">
         <v>6</v>
       </c>
@@ -779,8 +784,17 @@
       <c r="U4" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X4" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -822,7 +836,7 @@
       <c r="Q5" s="1">
         <v>30</v>
       </c>
-      <c r="R5" s="5"/>
+      <c r="R5" s="4"/>
       <c r="S5" s="1" t="s">
         <v>23</v>
       </c>
@@ -832,8 +846,17 @@
       <c r="U5" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X5" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -875,7 +898,7 @@
       <c r="Q6" s="1">
         <v>55</v>
       </c>
-      <c r="R6" s="5"/>
+      <c r="R6" s="4"/>
       <c r="S6" s="1" t="s">
         <v>59</v>
       </c>
@@ -885,8 +908,17 @@
       <c r="U6" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="X6" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -928,7 +960,7 @@
       <c r="Q7" s="1">
         <v>91</v>
       </c>
-      <c r="R7" s="5"/>
+      <c r="R7" s="4"/>
       <c r="S7" s="1" t="s">
         <v>35</v>
       </c>
@@ -938,8 +970,17 @@
       <c r="U7" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X7" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>23</v>
       </c>
@@ -975,7 +1016,7 @@
       <c r="Q8" s="1">
         <v>18</v>
       </c>
-      <c r="R8" s="5"/>
+      <c r="R8" s="4"/>
       <c r="S8" s="1" t="s">
         <v>38</v>
       </c>
@@ -985,8 +1026,17 @@
       <c r="U8" s="1">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X8" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -1022,7 +1072,7 @@
       <c r="Q9" s="1">
         <v>43</v>
       </c>
-      <c r="R9" s="5"/>
+      <c r="R9" s="4"/>
       <c r="S9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1032,8 +1082,17 @@
       <c r="U9" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X9" s="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>29</v>
       </c>
@@ -1069,7 +1128,7 @@
       <c r="Q10" s="1">
         <v>84</v>
       </c>
-      <c r="R10" s="5"/>
+      <c r="R10" s="4"/>
       <c r="S10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1079,8 +1138,17 @@
       <c r="U10" s="1">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X10" s="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>32</v>
       </c>
@@ -1116,7 +1184,7 @@
       <c r="Q11" s="1">
         <v>145</v>
       </c>
-      <c r="R11" s="5"/>
+      <c r="R11" s="4"/>
       <c r="S11" s="1" t="s">
         <v>60</v>
       </c>
@@ -1126,8 +1194,17 @@
       <c r="U11" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X11" s="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>35</v>
       </c>
@@ -1163,7 +1240,7 @@
       <c r="Q12" s="1">
         <v>38</v>
       </c>
-      <c r="R12" s="5"/>
+      <c r="R12" s="4"/>
       <c r="S12" s="1" t="s">
         <v>41</v>
       </c>
@@ -1173,8 +1250,17 @@
       <c r="U12" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X12" s="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>41</v>
       </c>
@@ -1210,7 +1296,7 @@
       <c r="Q13" s="1">
         <v>70</v>
       </c>
-      <c r="R13" s="5"/>
+      <c r="R13" s="4"/>
       <c r="S13" s="1" t="s">
         <v>44</v>
       </c>
@@ -1220,8 +1306,17 @@
       <c r="U13" s="1">
         <v>70</v>
       </c>
-    </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X13" s="1">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>47</v>
       </c>
@@ -1257,18 +1352,9 @@
       <c r="Q14" s="1">
         <v>120</v>
       </c>
-      <c r="R14" s="5"/>
-      <c r="S14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U14" s="1">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>53</v>
       </c>
@@ -1304,18 +1390,9 @@
       <c r="Q15" s="1">
         <v>192</v>
       </c>
-      <c r="R15" s="5"/>
-      <c r="S15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U15" s="1">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>38</v>
       </c>
@@ -1351,18 +1428,9 @@
       <c r="Q16" s="1">
         <v>14</v>
       </c>
-      <c r="R16" s="5"/>
-      <c r="S16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="U16" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>44</v>
       </c>
@@ -1398,18 +1466,9 @@
       <c r="Q17" s="1">
         <v>30</v>
       </c>
-      <c r="R17" s="5"/>
-      <c r="S17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U17" s="1">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>50</v>
       </c>
@@ -1445,18 +1504,9 @@
       <c r="Q18" s="1">
         <v>64</v>
       </c>
-      <c r="R18" s="5"/>
-      <c r="S18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="U18" s="1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>56</v>
       </c>
@@ -1492,18 +1542,9 @@
       <c r="Q19" s="1">
         <v>109</v>
       </c>
-      <c r="R19" s="5"/>
-      <c r="S19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U19" s="1">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="R19" s="4"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>59</v>
       </c>
@@ -1545,18 +1586,9 @@
       <c r="Q20" s="1">
         <v>24</v>
       </c>
-      <c r="R20" s="5"/>
-      <c r="S20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U20" s="1">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="R20" s="4"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>60</v>
       </c>
@@ -1598,18 +1630,9 @@
       <c r="Q21" s="1">
         <v>45</v>
       </c>
-      <c r="R21" s="5"/>
-      <c r="S21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="U21" s="1">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="R21" s="4"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>61</v>
       </c>
@@ -1651,18 +1674,9 @@
       <c r="Q22" s="1">
         <v>84</v>
       </c>
-      <c r="R22" s="5"/>
-      <c r="S22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="U22" s="1">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="R22" s="4"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>63</v>
       </c>
@@ -1704,16 +1718,7 @@
       <c r="Q23" s="1">
         <v>131</v>
       </c>
-      <c r="R23" s="5"/>
-      <c r="S23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="U23" s="1">
-        <v>192</v>
-      </c>
+      <c r="R23" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
extrapolation of indiv energies and 2nd revision data (#5)
* FEAT: add code to extrapolate correlation energies only or RHF/UHF data separately

* DATA: add extrapolations for full ds

* DATA: data for 2nd revision

* GIT: fix merge
</commit_message>
<xml_diff>
--- a/data/basisSetSizes.xlsx
+++ b/data/basisSetSizes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morgunov/vv/cebe_prediction/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morgunov/vv/cebe_prediction/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63B6D92-DEA1-2D4B-AD90-47BBCE585C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5AB5EE-4200-1540-8979-470B9946B46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="73">
   <si>
     <t>H</t>
   </si>
@@ -246,6 +246,12 @@
   </si>
   <si>
     <t># Func</t>
+  </si>
+  <si>
+    <t>Num. Functions</t>
+  </si>
+  <si>
+    <t>Contraction</t>
   </si>
 </sst>
 </file>
@@ -282,7 +288,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -305,24 +311,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -663,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:V23"/>
+  <dimension ref="B3:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3:X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -680,17 +676,18 @@
     <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.6640625" customWidth="1"/>
     <col min="20" max="20" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="C3" s="6" t="s">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="6"/>
       <c r="I3" s="2" t="s">
         <v>2</v>
       </c>
@@ -715,19 +712,27 @@
       <c r="Q3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="R3" s="4"/>
+      <c r="R3" s="3"/>
       <c r="S3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="V3" s="3"/>
-    </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -769,7 +774,7 @@
       <c r="Q4" s="1">
         <v>14</v>
       </c>
-      <c r="R4" s="5"/>
+      <c r="R4" s="4"/>
       <c r="S4" s="1" t="s">
         <v>6</v>
       </c>
@@ -779,8 +784,17 @@
       <c r="U4" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X4" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -822,7 +836,7 @@
       <c r="Q5" s="1">
         <v>30</v>
       </c>
-      <c r="R5" s="5"/>
+      <c r="R5" s="4"/>
       <c r="S5" s="1" t="s">
         <v>23</v>
       </c>
@@ -832,8 +846,17 @@
       <c r="U5" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X5" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -875,7 +898,7 @@
       <c r="Q6" s="1">
         <v>55</v>
       </c>
-      <c r="R6" s="5"/>
+      <c r="R6" s="4"/>
       <c r="S6" s="1" t="s">
         <v>59</v>
       </c>
@@ -885,8 +908,17 @@
       <c r="U6" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="X6" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -928,7 +960,7 @@
       <c r="Q7" s="1">
         <v>91</v>
       </c>
-      <c r="R7" s="5"/>
+      <c r="R7" s="4"/>
       <c r="S7" s="1" t="s">
         <v>35</v>
       </c>
@@ -938,8 +970,17 @@
       <c r="U7" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X7" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>23</v>
       </c>
@@ -975,7 +1016,7 @@
       <c r="Q8" s="1">
         <v>18</v>
       </c>
-      <c r="R8" s="5"/>
+      <c r="R8" s="4"/>
       <c r="S8" s="1" t="s">
         <v>38</v>
       </c>
@@ -985,8 +1026,17 @@
       <c r="U8" s="1">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X8" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -1022,7 +1072,7 @@
       <c r="Q9" s="1">
         <v>43</v>
       </c>
-      <c r="R9" s="5"/>
+      <c r="R9" s="4"/>
       <c r="S9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1032,8 +1082,17 @@
       <c r="U9" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X9" s="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>29</v>
       </c>
@@ -1069,7 +1128,7 @@
       <c r="Q10" s="1">
         <v>84</v>
       </c>
-      <c r="R10" s="5"/>
+      <c r="R10" s="4"/>
       <c r="S10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1079,8 +1138,17 @@
       <c r="U10" s="1">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X10" s="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>32</v>
       </c>
@@ -1116,7 +1184,7 @@
       <c r="Q11" s="1">
         <v>145</v>
       </c>
-      <c r="R11" s="5"/>
+      <c r="R11" s="4"/>
       <c r="S11" s="1" t="s">
         <v>60</v>
       </c>
@@ -1126,8 +1194,17 @@
       <c r="U11" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X11" s="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>35</v>
       </c>
@@ -1163,7 +1240,7 @@
       <c r="Q12" s="1">
         <v>38</v>
       </c>
-      <c r="R12" s="5"/>
+      <c r="R12" s="4"/>
       <c r="S12" s="1" t="s">
         <v>41</v>
       </c>
@@ -1173,8 +1250,17 @@
       <c r="U12" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X12" s="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>41</v>
       </c>
@@ -1210,7 +1296,7 @@
       <c r="Q13" s="1">
         <v>70</v>
       </c>
-      <c r="R13" s="5"/>
+      <c r="R13" s="4"/>
       <c r="S13" s="1" t="s">
         <v>44</v>
       </c>
@@ -1220,8 +1306,17 @@
       <c r="U13" s="1">
         <v>70</v>
       </c>
-    </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X13" s="1">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>47</v>
       </c>
@@ -1257,18 +1352,9 @@
       <c r="Q14" s="1">
         <v>120</v>
       </c>
-      <c r="R14" s="5"/>
-      <c r="S14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U14" s="1">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>53</v>
       </c>
@@ -1304,18 +1390,9 @@
       <c r="Q15" s="1">
         <v>192</v>
       </c>
-      <c r="R15" s="5"/>
-      <c r="S15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U15" s="1">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>38</v>
       </c>
@@ -1351,18 +1428,9 @@
       <c r="Q16" s="1">
         <v>14</v>
       </c>
-      <c r="R16" s="5"/>
-      <c r="S16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="U16" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>44</v>
       </c>
@@ -1398,18 +1466,9 @@
       <c r="Q17" s="1">
         <v>30</v>
       </c>
-      <c r="R17" s="5"/>
-      <c r="S17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U17" s="1">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>50</v>
       </c>
@@ -1445,18 +1504,9 @@
       <c r="Q18" s="1">
         <v>64</v>
       </c>
-      <c r="R18" s="5"/>
-      <c r="S18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="U18" s="1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>56</v>
       </c>
@@ -1492,18 +1542,9 @@
       <c r="Q19" s="1">
         <v>109</v>
       </c>
-      <c r="R19" s="5"/>
-      <c r="S19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U19" s="1">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="R19" s="4"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>59</v>
       </c>
@@ -1545,18 +1586,9 @@
       <c r="Q20" s="1">
         <v>24</v>
       </c>
-      <c r="R20" s="5"/>
-      <c r="S20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U20" s="1">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="R20" s="4"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>60</v>
       </c>
@@ -1598,18 +1630,9 @@
       <c r="Q21" s="1">
         <v>45</v>
       </c>
-      <c r="R21" s="5"/>
-      <c r="S21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="U21" s="1">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="R21" s="4"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>61</v>
       </c>
@@ -1651,18 +1674,9 @@
       <c r="Q22" s="1">
         <v>84</v>
       </c>
-      <c r="R22" s="5"/>
-      <c r="S22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="U22" s="1">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="R22" s="4"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>63</v>
       </c>
@@ -1704,16 +1718,7 @@
       <c r="Q23" s="1">
         <v>131</v>
       </c>
-      <c r="R23" s="5"/>
-      <c r="S23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="U23" s="1">
-        <v>192</v>
-      </c>
+      <c r="R23" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>